<commit_message>
alterei a porra toda, imagens e planilha.. agora ta tudo certinho
</commit_message>
<xml_diff>
--- a/Planilha sismica.xlsx
+++ b/Planilha sismica.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Arquivo</t>
   </si>
@@ -36,64 +36,109 @@
     <t>Δprof</t>
   </si>
   <si>
-    <t>11614°24.06000'S</t>
-  </si>
-  <si>
-    <t>11614°23.40000'S</t>
-  </si>
-  <si>
-    <t>11614°09.66000'S</t>
-  </si>
-  <si>
-    <t>11614°12.36000'S</t>
-  </si>
-  <si>
-    <t>11613°51.90000'S</t>
-  </si>
-  <si>
-    <t>11613°59.46000'S</t>
-  </si>
-  <si>
-    <t>11613°37.62000'S</t>
-  </si>
-  <si>
-    <t>11613°42.30000'S</t>
-  </si>
-  <si>
-    <t>11613°24.60000'S</t>
-  </si>
-  <si>
-    <t>11613°29.28000'S</t>
-  </si>
-  <si>
-    <t>218681°03.90000'W</t>
-  </si>
-  <si>
-    <t>218679°15.48000'W</t>
-  </si>
-  <si>
-    <t>218677°50.70000'W</t>
-  </si>
-  <si>
-    <t>218675°57.66000'W</t>
-  </si>
-  <si>
-    <t>218674°35.40000'W</t>
-  </si>
-  <si>
-    <t>218672°50.52000'W</t>
-  </si>
-  <si>
-    <t>218671°29.88000'W</t>
-  </si>
-  <si>
-    <t>218669°36.72000'W</t>
-  </si>
-  <si>
-    <t>218668°12.18000'W</t>
-  </si>
-  <si>
-    <t>218682°32.22000'W</t>
+    <t>03°1357438'S</t>
+  </si>
+  <si>
+    <t>060°4470898'W</t>
+  </si>
+  <si>
+    <t>03°1357420'S</t>
+  </si>
+  <si>
+    <t>03°1356935'S</t>
+  </si>
+  <si>
+    <t>03°1357010'S</t>
+  </si>
+  <si>
+    <t>03°1356441'S</t>
+  </si>
+  <si>
+    <t>03°1356651'S</t>
+  </si>
+  <si>
+    <t>03°1356175'S</t>
+  </si>
+  <si>
+    <t>03°1355570'S</t>
+  </si>
+  <si>
+    <t>03°1355728'S</t>
+  </si>
+  <si>
+    <t>060°4465430'W</t>
+  </si>
+  <si>
+    <t>060°4463075'W</t>
+  </si>
+  <si>
+    <t>060°4459935'W</t>
+  </si>
+  <si>
+    <t>060°4457650'W</t>
+  </si>
+  <si>
+    <t>060°4454736'W</t>
+  </si>
+  <si>
+    <t>060°4449363'W</t>
+  </si>
+  <si>
+    <t>060°4446981'W</t>
+  </si>
+  <si>
+    <t>060°4452496'W</t>
+  </si>
+  <si>
+    <t>Todos com correção de +1 m</t>
+  </si>
+  <si>
+    <t>20150630135215-1</t>
+  </si>
+  <si>
+    <t>20150630135446-1</t>
+  </si>
+  <si>
+    <t>20150610135803-1</t>
+  </si>
+  <si>
+    <t>20150610140033-1</t>
+  </si>
+  <si>
+    <t>20150610140338-1</t>
+  </si>
+  <si>
+    <t>03°1345788'S</t>
+  </si>
+  <si>
+    <t>03°1356045'S</t>
+  </si>
+  <si>
+    <t>03°1345694'S</t>
+  </si>
+  <si>
+    <t>03°1346184'S</t>
+  </si>
+  <si>
+    <t>03°1346061'S</t>
+  </si>
+  <si>
+    <t>03°1346586'S</t>
+  </si>
+  <si>
+    <t>060°4315981'W</t>
+  </si>
+  <si>
+    <t>060°4317778'W</t>
+  </si>
+  <si>
+    <t>060°4321206'W</t>
+  </si>
+  <si>
+    <t>060°4323378'W</t>
+  </si>
+  <si>
+    <t>060°4326421'W</t>
   </si>
 </sst>
 </file>
@@ -103,7 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +157,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -140,18 +193,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -449,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -462,227 +521,335 @@
     <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3">
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1">
+        <v>17.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>17.3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E6" s="1">
+        <v>17.7</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
         <v>20150701160615</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="1">
-        <v>15.6</v>
-      </c>
-      <c r="E2" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4">
-        <v>20150701160906</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="1">
-        <v>15.6</v>
-      </c>
-      <c r="E3" s="1">
-        <v>15.9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4">
-        <v>20150701161147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1">
-        <v>15.6</v>
-      </c>
-      <c r="E4" s="1">
-        <v>15.8</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4">
-        <v>20150701161518</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1">
-        <v>15.5</v>
-      </c>
-      <c r="E5" s="1">
-        <v>16</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4">
-        <v>20150701161749</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1">
-        <v>15.5</v>
-      </c>
-      <c r="E6" s="1">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4">
-        <v>20150701162047</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" s="1">
-        <v>15.4</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>15.6</v>
+        <v>16.8</v>
       </c>
       <c r="F7" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4">
-        <v>20150701162348</v>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3">
+        <v>20150701160906</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1">
-        <v>15.7</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="E8" s="1">
-        <v>15.8</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="F8" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4">
-        <v>20150701162647</v>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3">
+        <v>20150701161147</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1">
-        <v>15.5</v>
+        <v>16.7</v>
       </c>
       <c r="E9" s="1">
-        <v>15.7</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="F9" s="1">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4">
+    <row r="10" spans="1:10">
+      <c r="A10" s="3">
+        <v>20150701161518</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3">
+        <v>20150701161749</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>17</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3">
+        <v>20150701162047</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3">
+        <v>20150701162348</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="E13" s="1">
+        <v>16.8</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3">
+        <v>20150701162647</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3">
         <v>20150701162934</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="1">
-        <v>15.4</v>
-      </c>
-      <c r="E10" s="1">
-        <v>15.6</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4">
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="E15" s="1">
+        <v>16.7</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3">
         <v>20150701163228</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1">
-        <v>15.3</v>
-      </c>
-      <c r="E11" s="1">
-        <v>15.4</v>
-      </c>
-      <c r="F11" s="1">
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E16" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="F16" s="1">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>